<commit_message>
Model cleanup, documentation of parameters + functions in main, KpiVisuals
-Obsolete parameters verwijderd uit het model en brondata
-Documentatie toegevoegd voor parameters en functies etc. in main, KpiVisuals.
</commit_message>
<xml_diff>
--- a/Base/db_backboneParams.xlsx
+++ b/Base/db_backboneParams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C679BE79-0D9D-4DBE-8392-73242D8942D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85157A78-1F3F-4F6F-B9FD-0FC85707E107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>index</t>
   </si>
@@ -59,45 +59,6 @@
   </si>
   <si>
     <t>p_timeStep_h</t>
-  </si>
-  <si>
-    <t>p_houseOtherElectricityDemandPeak_kW</t>
-  </si>
-  <si>
-    <t>kW</t>
-  </si>
-  <si>
-    <t>p_storeOtherElectricityDemandPeak_kW</t>
-  </si>
-  <si>
-    <t>p_officeOtherElectricityDemandPeak_kW</t>
-  </si>
-  <si>
-    <t>Peak power demand for lighting, devices. To be scaled by profile</t>
-  </si>
-  <si>
-    <t>House GasBurner peak thermal delivery in kW</t>
-  </si>
-  <si>
-    <t>p_houseGasBurnerThermalCapacity_kW</t>
-  </si>
-  <si>
-    <t>p_houseGasBurnerEfficiency_r</t>
-  </si>
-  <si>
-    <t>Residential gas burner efficiency</t>
-  </si>
-  <si>
-    <t>p_houseHeatPumpEfficiency_r</t>
-  </si>
-  <si>
-    <t>Residential heatPump efficiency (COP = 3)</t>
-  </si>
-  <si>
-    <t>p_houseHeatPumpElectricCapacity_kW</t>
-  </si>
-  <si>
-    <t>Average residential heatpump electrical power</t>
   </si>
   <si>
     <t>p_undergroundTemperature_degC</t>
@@ -421,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,123 +435,10 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>0.95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'f_updateincentives' to connectionOwners
A connection owner now has a dynamic electricity price variable and an 'excess electricity' (energy balance) variable, that can be used by controllers of flex-assets.
</commit_message>
<xml_diff>
--- a/Base/db_backboneParams.xlsx
+++ b/Base/db_backboneParams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE02DBEE-BD97-4A6D-9296-CC2C881B44E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523B979-F530-422D-9D1B-CB54BF2618DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Agent population data, fix timeStep-setting
-ExperimentSettings bevat nu ook data voor aantallen agents per type ter check
-TimeStep is uit de lokale excel-file gehaald zodat deze niet meer overschrijft wat wordt ingesteld vanuit het experiment.
</commit_message>
<xml_diff>
--- a/Base/db_backboneParams.xlsx
+++ b/Base/db_backboneParams.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523B979-F530-422D-9D1B-CB54BF2618DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA65D36-CE74-4762-A088-5F376814426E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>index</t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>simulation timestep in hours</t>
-  </si>
-  <si>
-    <t>p_timeStep_h</t>
   </si>
   <si>
     <t>p_undergroundTemperature_degC</t>
@@ -382,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,30 +406,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0.25</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes contracts, hybrid heatpumps, nested energy holons
Fixes contracts, hybrid heatpumps, nested energy holons
</commit_message>
<xml_diff>
--- a/Base/db_backboneParams.xlsx
+++ b/Base/db_backboneParams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC841C6F-089E-4EE8-A4D9-E6F356206004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282C40E4-872E-4E56-909B-FDBB354BDF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>